<commit_message>
03/04/2021 09:46 | started notebook, major changes upcoming, see changelog
</commit_message>
<xml_diff>
--- a/target_workbook.xlsx
+++ b/target_workbook.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesmacdonald/Dropbox/Box Sync/code/fidelityReview/fidelity-portfolio-review/fidelity-portfolio-review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61629BA0-6689-AF49-B2B8-B60FB8EFCF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CBFC55-0894-F743-8EE9-D149D9215A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34420" yWindow="3380" windowWidth="29000" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Portfolio_Position_Nov-01-2020" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6695,7 +6695,7 @@
   <dimension ref="A1:AM114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="X2" sqref="X2"/>

</xml_diff>